<commit_message>
GBDS JANUARY FILES 2026 - fliqlo@GBDS
</commit_message>
<xml_diff>
--- a/GBDS JANUARY FILES 2026/CSR MONTH OF JANUARY 2026.xlsx
+++ b/GBDS JANUARY FILES 2026/CSR MONTH OF JANUARY 2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS JANUARY FILES 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702040EE-0AEE-4D9E-82E1-FE23127B4F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8DD3DA-ED81-40AC-A9C5-E9659D09C16A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="24" activeTab="36" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | JANUARY" sheetId="902" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="01-01 R2" sheetId="1106" r:id="rId4"/>
     <sheet name="01-01 R3" sheetId="1107" r:id="rId5"/>
     <sheet name="(2)" sheetId="1218" r:id="rId6"/>
-    <sheet name="01-02 R1" sheetId="1219" r:id="rId7"/>
-    <sheet name="01-02 R2" sheetId="1220" r:id="rId8"/>
+    <sheet name="01-02 R1 NO TRIP" sheetId="1219" r:id="rId7"/>
+    <sheet name="01-02 R2 NO TRIP" sheetId="1220" r:id="rId8"/>
     <sheet name="01-02 R3" sheetId="1221" r:id="rId9"/>
     <sheet name="(3)" sheetId="1222" r:id="rId10"/>
     <sheet name="01-03 R1" sheetId="1223" r:id="rId11"/>
@@ -69,8 +69,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'01-01 R1'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'01-01 R2'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'01-01 R3'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'01-02 R1'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'01-02 R2'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'01-02 R1 NO TRIP'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'01-02 R2 NO TRIP'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'01-02 R3'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'01-03 R1'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'01-03 R2'!$A$1:$V$44</definedName>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="77">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>DATE ___________01/10/2026___________</t>
+  </si>
+  <si>
+    <t>4/18B</t>
+  </si>
+  <si>
+    <t>13/6B</t>
   </si>
 </sst>
 </file>
@@ -46116,7 +46122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30C8572-145E-439B-B149-FD0C598987C7}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -56481,7 +56487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F9F6FB-C769-4F8B-9761-4E622DA4D608}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -56835,12 +56841,20 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>4</v>
+      </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15">
+        <v>18</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -56852,9 +56866,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -57002,12 +57020,20 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>4</v>
+      </c>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>76</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -57019,20 +57045,32 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>2</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>75</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -57044,9 +57082,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -57429,20 +57471,34 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>137</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>20</v>
+      </c>
+      <c r="N24" s="15">
+        <v>482</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>20</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
+      <c r="U24" s="15">
+        <v>8</v>
+      </c>
       <c r="V24" s="16"/>
     </row>
     <row r="25" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57594,20 +57650,34 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>62</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>2</v>
+      </c>
+      <c r="M31" s="24">
+        <v>8</v>
+      </c>
+      <c r="N31" s="24">
+        <v>2</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>20</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
-      <c r="U31" s="64"/>
+      <c r="U31" s="64">
+        <v>0</v>
+      </c>
       <c r="V31" s="25"/>
     </row>
     <row r="32" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -57619,20 +57689,34 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>75</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>12</v>
+      </c>
+      <c r="N32" s="29">
+        <v>480</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
-      <c r="U32" s="66"/>
+      <c r="U32" s="66">
+        <v>8</v>
+      </c>
       <c r="V32" s="30"/>
     </row>
     <row r="33" spans="2:23" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -57754,21 +57838,47 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="F36" s="45">
+        <v>680</v>
+      </c>
+      <c r="G36" s="45">
+        <v>2</v>
+      </c>
+      <c r="H36" s="45">
+        <v>21</v>
+      </c>
+      <c r="I36" s="45">
+        <v>6</v>
+      </c>
+      <c r="J36" s="45">
+        <v>6</v>
+      </c>
+      <c r="K36" s="45">
+        <v>14</v>
+      </c>
+      <c r="L36" s="45">
+        <v>4</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1</v>
+      </c>
+      <c r="N36" s="45">
+        <v>6</v>
+      </c>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>24</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -57894,21 +58004,47 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="F42" s="45">
+        <v>680</v>
+      </c>
+      <c r="G42" s="45">
+        <v>2</v>
+      </c>
+      <c r="H42" s="45">
+        <v>21</v>
+      </c>
+      <c r="I42" s="45">
+        <v>6</v>
+      </c>
+      <c r="J42" s="45">
+        <v>6</v>
+      </c>
+      <c r="K42" s="45">
+        <v>14</v>
+      </c>
+      <c r="L42" s="45">
+        <v>4</v>
+      </c>
+      <c r="M42" s="45">
+        <v>1</v>
+      </c>
+      <c r="N42" s="45">
+        <v>6</v>
+      </c>
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>24</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
GBDS JANUARY FILES 2026 | fliqlo@GBDS
</commit_message>
<xml_diff>
--- a/GBDS JANUARY FILES 2026/CSR MONTH OF JANUARY 2026.xlsx
+++ b/GBDS JANUARY FILES 2026/CSR MONTH OF JANUARY 2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS JANUARY FILES 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0468F404-C9F4-46A1-8A76-2D3C7C63183A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78089DEE-45B0-4BBE-991E-A5361CFD2871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="16" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="20" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | JANUARY" sheetId="902" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="101">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -383,6 +383,36 @@
   </si>
   <si>
     <t>24/6B</t>
+  </si>
+  <si>
+    <t>19/3B</t>
+  </si>
+  <si>
+    <t>28/3B</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>1/12B</t>
+  </si>
+  <si>
+    <t>17/1B</t>
+  </si>
+  <si>
+    <t>20B</t>
+  </si>
+  <si>
+    <t>17/21B</t>
+  </si>
+  <si>
+    <t>22/18B</t>
+  </si>
+  <si>
+    <t>20/10B</t>
+  </si>
+  <si>
+    <t>2/8B</t>
   </si>
 </sst>
 </file>
@@ -943,7 +973,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1179,6 +1209,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -13987,7 +14020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8C24C4-CA38-4534-B5B2-1BF5BB250212}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -17431,11 +17464,15 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -17447,9 +17484,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>1</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -17598,11 +17639,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -17614,20 +17659,28 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24" t="s">
+        <v>93</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="77">
+        <v>9</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -17639,9 +17692,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59" t="s">
+        <v>93</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -18020,20 +18077,36 @@
         <v>23</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>1</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="J24" s="15">
+        <v>40</v>
+      </c>
+      <c r="K24" s="15">
+        <v>1</v>
+      </c>
+      <c r="L24" s="15">
+        <v>1</v>
+      </c>
+      <c r="M24" s="15">
+        <v>5</v>
+      </c>
+      <c r="N24" s="15">
+        <v>665</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>17</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -18185,20 +18258,36 @@
         <v>25</v>
       </c>
       <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
+      <c r="D31" s="24">
+        <v>1</v>
+      </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="J31" s="24">
+        <v>13</v>
+      </c>
+      <c r="K31" s="24">
+        <v>1</v>
+      </c>
+      <c r="L31" s="24">
+        <v>0</v>
+      </c>
+      <c r="M31" s="24">
+        <v>3</v>
+      </c>
+      <c r="N31" s="24">
+        <v>32</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>17</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -18210,20 +18299,36 @@
         <v>26</v>
       </c>
       <c r="C32" s="27"/>
-      <c r="D32" s="28"/>
+      <c r="D32" s="28">
+        <v>0</v>
+      </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>1</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="J32" s="29">
+        <v>27</v>
+      </c>
+      <c r="K32" s="29">
+        <v>0</v>
+      </c>
+      <c r="L32" s="29">
+        <v>1</v>
+      </c>
+      <c r="M32" s="29">
+        <v>2</v>
+      </c>
+      <c r="N32" s="29">
+        <v>633</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -18352,18 +18457,40 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
+      <c r="F36" s="45">
+        <v>641</v>
+      </c>
+      <c r="G36" s="45">
+        <v>12</v>
+      </c>
+      <c r="H36" s="45">
+        <v>9</v>
+      </c>
+      <c r="I36" s="45">
+        <v>12</v>
+      </c>
+      <c r="J36" s="45">
+        <v>2</v>
+      </c>
+      <c r="K36" s="45">
+        <v>11</v>
+      </c>
+      <c r="L36" s="45">
+        <v>3</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1</v>
+      </c>
+      <c r="N36" s="45">
+        <v>3</v>
+      </c>
+      <c r="O36" s="45">
+        <v>6</v>
+      </c>
       <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="Q36" s="46">
+        <v>22</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -18492,18 +18619,40 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
+      <c r="F42" s="45">
+        <v>641</v>
+      </c>
+      <c r="G42" s="45">
+        <v>12</v>
+      </c>
+      <c r="H42" s="45">
+        <v>9</v>
+      </c>
+      <c r="I42" s="45">
+        <v>12</v>
+      </c>
+      <c r="J42" s="45">
+        <v>2</v>
+      </c>
+      <c r="K42" s="45">
+        <v>11</v>
+      </c>
+      <c r="L42" s="45">
+        <v>3</v>
+      </c>
+      <c r="M42" s="45">
+        <v>1</v>
+      </c>
+      <c r="N42" s="45">
+        <v>3</v>
+      </c>
+      <c r="O42" s="45">
+        <v>6</v>
+      </c>
       <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="Q42" s="46">
+        <v>22</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -20391,12 +20540,20 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14">
+        <v>4</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="15">
+        <v>3</v>
+      </c>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -20408,9 +20565,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -20558,12 +20719,20 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>3</v>
+      </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>96</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -20575,20 +20744,32 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>2</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="60">
+        <v>1</v>
+      </c>
       <c r="D16" s="61"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="F16" s="28">
+        <v>3</v>
+      </c>
+      <c r="G16" s="29">
+        <v>1</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -20600,9 +20781,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -20985,15 +21170,27 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>2</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>58</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>10</v>
+      </c>
+      <c r="N24" s="15">
+        <v>640</v>
+      </c>
       <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
+      <c r="P24" s="15">
+        <v>1</v>
+      </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
@@ -21150,15 +21347,27 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>2</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>17</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>2</v>
+      </c>
+      <c r="M31" s="24">
+        <v>7</v>
+      </c>
+      <c r="N31" s="24">
+        <v>59</v>
+      </c>
       <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
+      <c r="P31" s="24">
+        <v>0</v>
+      </c>
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
@@ -21175,15 +21384,27 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>41</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>3</v>
+      </c>
+      <c r="N32" s="29">
+        <v>581</v>
+      </c>
       <c r="O32" s="24"/>
-      <c r="P32" s="29"/>
+      <c r="P32" s="29">
+        <v>1</v>
+      </c>
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
@@ -21313,18 +21534,38 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="F36" s="45">
+        <v>758</v>
+      </c>
+      <c r="G36" s="45">
+        <v>1</v>
+      </c>
       <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+      <c r="I36" s="45">
+        <v>2</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>2</v>
+      </c>
+      <c r="L36" s="45">
+        <v>3</v>
+      </c>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>24</v>
+      </c>
+      <c r="O36" s="45">
+        <v>8</v>
+      </c>
+      <c r="P36" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>21</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -21453,18 +21694,38 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="F42" s="45">
+        <v>758</v>
+      </c>
+      <c r="G42" s="45">
+        <v>1</v>
+      </c>
       <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
+      <c r="I42" s="45">
+        <v>2</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>2</v>
+      </c>
+      <c r="L42" s="45">
+        <v>3</v>
+      </c>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="N42" s="45">
+        <v>24</v>
+      </c>
+      <c r="O42" s="45">
+        <v>8</v>
+      </c>
+      <c r="P42" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>21</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -21518,7 +21779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C68E2D-4089-4CE9-8E40-AA436510A840}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -21872,12 +22133,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15">
+        <v>3</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -21889,9 +22156,15 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
+      <c r="U8" s="62">
+        <v>1</v>
+      </c>
+      <c r="V8" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -22039,12 +22312,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>2</v>
+      </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="F15" s="24">
+        <v>2</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>99</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -22056,20 +22335,32 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="T15" s="24">
+        <v>2</v>
+      </c>
+      <c r="U15" s="64">
+        <v>0</v>
+      </c>
+      <c r="V15" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
       <c r="D16" s="61"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -22081,9 +22372,15 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
-      <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
+      <c r="U16" s="65">
+        <v>1</v>
+      </c>
+      <c r="V16" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -22461,21 +22758,37 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>2</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="J24" s="15">
+        <v>130</v>
+      </c>
+      <c r="K24" s="15">
+        <v>1</v>
+      </c>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>20</v>
+      </c>
+      <c r="N24" s="15">
+        <v>614</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>18</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -22626,21 +22939,37 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>2</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="J31" s="24">
+        <v>117</v>
+      </c>
+      <c r="K31" s="24">
+        <v>1</v>
+      </c>
+      <c r="L31" s="24">
+        <v>2</v>
+      </c>
+      <c r="M31" s="24">
+        <v>19</v>
+      </c>
+      <c r="N31" s="24">
+        <v>273</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>18</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -22651,21 +22980,37 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>0</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="J32" s="29">
+        <v>13</v>
+      </c>
+      <c r="K32" s="29">
+        <v>0</v>
+      </c>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>1</v>
+      </c>
+      <c r="N32" s="29">
+        <v>341</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -22791,21 +23136,47 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
       <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+      <c r="E36" s="45">
+        <v>1</v>
+      </c>
+      <c r="F36" s="45">
+        <v>439</v>
+      </c>
+      <c r="G36" s="45">
+        <v>3</v>
+      </c>
+      <c r="H36" s="45">
+        <v>2</v>
+      </c>
+      <c r="I36" s="45">
+        <v>25</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>11</v>
+      </c>
+      <c r="L36" s="45">
+        <v>2</v>
+      </c>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>7</v>
+      </c>
+      <c r="O36" s="45">
+        <v>1</v>
+      </c>
+      <c r="P36" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>16</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -22931,21 +23302,47 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
       <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
+      <c r="E42" s="45">
+        <v>1</v>
+      </c>
+      <c r="F42" s="45">
+        <v>439</v>
+      </c>
+      <c r="G42" s="45">
+        <v>3</v>
+      </c>
+      <c r="H42" s="45">
+        <v>2</v>
+      </c>
+      <c r="I42" s="45">
+        <v>25</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>11</v>
+      </c>
+      <c r="L42" s="45">
+        <v>2</v>
+      </c>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="N42" s="45">
+        <v>7</v>
+      </c>
+      <c r="O42" s="45">
+        <v>1</v>
+      </c>
+      <c r="P42" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>16</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>

</xml_diff>